<commit_message>
Remove outliers with extreme offsets
</commit_message>
<xml_diff>
--- a/analysis/a_priori_power/EffectSizes.xlsx
+++ b/analysis/a_priori_power/EffectSizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebET\30_dataAnalysis\APrioriPower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\GitHub\WebET_Analysis\analysis\a_priori_power\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76877E39-A15E-476D-9211-BA6F64332622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D651558-71CC-464B-A450-102A138EBCEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle3" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Factor</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Degree</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1086,13 +1089,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>43</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>-4.8199999999999993E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -1116,13 +1119,13 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>6.17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>0.74399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>0.49792011120817498</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
@@ -1185,29 +1188,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="2"/>
-    <col min="3" max="3" width="8.7265625" style="13"/>
-    <col min="4" max="4" width="8.7265625" style="2"/>
-    <col min="5" max="5" width="8.7265625" style="13"/>
-    <col min="6" max="6" width="13.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="19"/>
-    <col min="8" max="8" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="15.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="2"/>
+    <col min="3" max="3" width="8.77734375" style="13"/>
+    <col min="4" max="4" width="8.77734375" style="2"/>
+    <col min="5" max="5" width="8.77734375" style="13"/>
+    <col min="6" max="6" width="13.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="19"/>
+    <col min="8" max="8" width="8.77734375" style="2"/>
     <col min="9" max="9" width="17" style="2" customWidth="1"/>
     <col min="10" max="10" width="22" style="2" customWidth="1"/>
-    <col min="11" max="11" width="34.26953125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="34.21875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>0.47874847091992484</v>
       </c>
       <c r="F3" s="15">
-        <f t="shared" ref="F3:F18" si="0">TAN(C3*PI()/180)*50</f>
+        <f t="shared" ref="F3:F19" si="0">TAN(C3*PI()/180)*50</f>
         <v>0.35727497829845134</v>
       </c>
       <c r="G3" s="17">
@@ -1309,7 +1312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
@@ -1735,130 +1738,127 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
+    <row r="19" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>50</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="13">
-        <v>1</v>
-      </c>
-      <c r="F20" s="15">
-        <f>TAN(C20*PI()/180)*50</f>
-        <v>0.87275324641087926</v>
-      </c>
-      <c r="G20" s="19">
-        <f>(F20/38.1)*100</f>
-        <v>2.2906909354616252</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F21" s="15">
-        <f>TAN(C21*PI()/180)*50</f>
-        <v>0.43634338953793944</v>
+        <f t="shared" ref="F21:F29" si="9">TAN(C21*PI()/180)*50</f>
+        <v>0.87275324641087926</v>
       </c>
       <c r="G21" s="19">
-        <f>(F21/38.1)*100</f>
-        <v>1.1452582402570588</v>
+        <f t="shared" ref="G21:G29" si="10">(F21/38.1)*100</f>
+        <v>2.2906909354616252</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="13">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F22" s="15">
-        <f>TAN(C22*PI()/180)*50</f>
-        <v>0.96004904538617497</v>
+        <f t="shared" si="9"/>
+        <v>0.43634338953793944</v>
       </c>
       <c r="G22" s="19">
-        <f>(F22/38.1)*100</f>
-        <v>2.5198137674177818</v>
+        <f t="shared" si="10"/>
+        <v>1.1452582402570588</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="13">
-        <v>0.77</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F23" s="15">
-        <f>TAN(C23*PI()/180)*50</f>
-        <v>0.6719922181541198</v>
+        <f t="shared" si="9"/>
+        <v>0.96004904538617497</v>
       </c>
       <c r="G23" s="19">
-        <f>(F23/38.1)*100</f>
-        <v>1.7637591027667185</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>2.5198137674177818</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="13">
-        <v>0.8</v>
+        <v>0.77</v>
       </c>
       <c r="F24" s="15">
-        <f>TAN(C24*PI()/180)*50</f>
-        <v>0.69817707245908267</v>
+        <f t="shared" si="9"/>
+        <v>0.6719922181541198</v>
       </c>
       <c r="G24" s="19">
-        <f>(F24/38.1)*100</f>
-        <v>1.8324857544857811</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="10"/>
+        <v>1.7637591027667185</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="13">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F25" s="15">
-        <f>TAN(C25*PI()/180)*50</f>
-        <v>0.87275324641087926</v>
+        <f t="shared" si="9"/>
+        <v>0.69817707245908267</v>
       </c>
       <c r="G25" s="19">
-        <f>(F25/38.1)*100</f>
-        <v>2.2906909354616252</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>27</v>
+        <f t="shared" si="10"/>
+        <v>1.8324857544857811</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1866,52 +1866,74 @@
         <v>1</v>
       </c>
       <c r="F26" s="15">
-        <f>TAN(C26*PI()/180)*50</f>
+        <f t="shared" si="9"/>
         <v>0.87275324641087926</v>
       </c>
       <c r="G26" s="19">
-        <f>(F26/38.1)*100</f>
+        <f t="shared" si="10"/>
         <v>2.2906909354616252</v>
       </c>
+      <c r="I26" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="K26" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="13">
+        <v>1</v>
+      </c>
+      <c r="F27" s="15">
+        <f t="shared" si="9"/>
+        <v>0.87275324641087926</v>
+      </c>
+      <c r="G27" s="19">
+        <f t="shared" si="10"/>
+        <v>2.2906909354616252</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="F27" s="15">
-        <f>TAN(C27*PI()/180)*50</f>
-        <v>0.26180178028500634</v>
-      </c>
-      <c r="G27" s="19">
-        <f>(F27/38.1)*100</f>
-        <v>0.68714378027560719</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="F28" s="15">
+        <f t="shared" si="9"/>
+        <v>0.26180178028500634</v>
+      </c>
+      <c r="G28" s="19">
+        <f t="shared" si="10"/>
+        <v>0.68714378027560719</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="13">
         <v>0.63</v>
       </c>
-      <c r="F28" s="15">
-        <f>TAN(C28*PI()/180)*50</f>
+      <c r="F29" s="15">
+        <f t="shared" si="9"/>
         <v>0.54980087201832584</v>
       </c>
-      <c r="G28" s="19">
-        <f>(F28/38.1)*100</f>
+      <c r="G29" s="19">
+        <f t="shared" si="10"/>
         <v>1.443046908184582</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>